<commit_message>
CoownersTable rewrite method searchByUserField - now its universal method to search by any user Field refactor my test
</commit_message>
<xml_diff>
--- a/UsersBD.xlsx
+++ b/UsersBD.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="37">
   <si>
     <t>account_non_expired</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>ttttt</t>
   </si>
 </sst>
 </file>
@@ -551,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
         <v>34</v>
@@ -1235,13 +1238,13 @@
         <v>35</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O11" s="3">
         <v>1</v>

</xml_diff>